<commit_message>
update textbooks and slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22559D26-F9F3-9F48-8FA3-51740B6E0C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC268F-3A6B-2D41-877A-6A231AF93110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>Week</t>
   </si>
@@ -56,9 +56,6 @@
     <t>WEEK 1</t>
   </si>
   <si>
-    <t>Lecture 0: Course Overview and Introduction</t>
-  </si>
-  <si>
     <t>WEEK 2</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>01-reading.html</t>
   </si>
   <si>
-    <t>00-reading.html</t>
-  </si>
-  <si>
     <t>hw-01</t>
   </si>
   <si>
@@ -146,18 +140,12 @@
     <t>hw-10</t>
   </si>
   <si>
-    <t>00-course-overview</t>
-  </si>
-  <si>
     <t>Old</t>
   </si>
   <si>
     <t>Midterm 1</t>
   </si>
   <si>
-    <t>lab-01-review.html</t>
-  </si>
-  <si>
     <t>Tues, Aug 26</t>
   </si>
   <si>
@@ -294,6 +282,15 @@
   </si>
   <si>
     <t>hw-11</t>
+  </si>
+  <si>
+    <t>Lecture 1:  Introduction to Linear Models</t>
+  </si>
+  <si>
+    <t>01-introduction</t>
+  </si>
+  <si>
+    <t>lab-01.html</t>
   </si>
 </sst>
 </file>
@@ -671,7 +668,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -700,13 +697,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -714,48 +711,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2"/>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -763,28 +758,28 @@
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="18">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -793,28 +788,28 @@
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="18">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -823,28 +818,28 @@
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="18">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -853,28 +848,28 @@
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="18">
       <c r="A17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -884,29 +879,29 @@
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="18">
       <c r="A20" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -916,58 +911,58 @@
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="G21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="18">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -976,28 +971,28 @@
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1007,27 +1002,27 @@
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2"/>
       <c r="G30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1036,57 +1031,57 @@
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
       <c r="G33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E36" s="2"/>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1095,16 +1090,16 @@
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1113,28 +1108,28 @@
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add lecture 2 and reading
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBC268F-3A6B-2D41-877A-6A231AF93110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47FF83-9B0C-AA45-B5BB-F50FDB1172F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>Week</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Labs</t>
   </si>
   <si>
-    <t>01-reading.html</t>
-  </si>
-  <si>
     <t>hw-01</t>
   </si>
   <si>
@@ -290,7 +287,19 @@
     <t>01-introduction</t>
   </si>
   <si>
-    <t>lab-01.html</t>
+    <t>01-introduction.html</t>
+  </si>
+  <si>
+    <t>02-mles</t>
+  </si>
+  <si>
+    <t>Lecture 2: MLEs &amp; Projections</t>
+  </si>
+  <si>
+    <t>02-MLEs.html</t>
+  </si>
+  <si>
+    <t>lab01.html</t>
   </si>
 </sst>
 </file>
@@ -700,10 +709,10 @@
         <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -711,38 +720,44 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
         <v>82</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="2"/>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -750,7 +765,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -758,19 +773,19 @@
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -779,7 +794,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -788,19 +803,19 @@
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -809,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -818,19 +833,19 @@
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -839,7 +854,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -848,19 +863,19 @@
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -869,7 +884,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -879,20 +894,20 @@
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -901,7 +916,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -911,23 +926,23 @@
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="G21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -935,7 +950,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
@@ -944,16 +959,16 @@
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -962,7 +977,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -971,19 +986,19 @@
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -992,7 +1007,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1002,18 +1017,18 @@
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="2"/>
       <c r="G30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -1022,7 +1037,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1031,19 +1046,19 @@
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
       <c r="G33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -1052,27 +1067,27 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2"/>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36" s="2"/>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -1081,7 +1096,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1090,7 +1105,7 @@
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -1099,7 +1114,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1108,10 +1123,10 @@
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D41" s="2"/>
     </row>
@@ -1121,7 +1136,7 @@
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
@@ -1129,7 +1144,7 @@
         <v>20</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update schedule for the week
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBB6D65-251E-244C-B5E1-DA48649A1503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A7C44-83F8-DF4F-BAFA-C6D651863ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Week</t>
   </si>
@@ -302,16 +302,16 @@
     <t>02-mles.html</t>
   </si>
   <si>
-    <t>Lecture 4: Linear Unbiased Estimation and Gauss-Markov</t>
-  </si>
-  <si>
     <t>03-non-full-rank</t>
   </si>
   <si>
-    <t>04-Gauss-Markov04-Gauss-Markov</t>
-  </si>
-  <si>
     <t>Lecture 3: Rank Deficient Models</t>
+  </si>
+  <si>
+    <t>Lecture 4: Best Linear Unbiased Estimation and Gauss-Markov Theorem</t>
+  </si>
+  <si>
+    <t>04-BLUE</t>
   </si>
 </sst>
 </file>
@@ -689,7 +689,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -780,13 +780,13 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
@@ -795,12 +795,14 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>91</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
update schedule and reading
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A7C44-83F8-DF4F-BAFA-C6D651863ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E77A0-A33D-FE4E-88C3-5F40B09780F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>Week</t>
   </si>
@@ -312,6 +312,24 @@
   </si>
   <si>
     <t>04-BLUE</t>
+  </si>
+  <si>
+    <t>Lecture 7: Sampling Distributions</t>
+  </si>
+  <si>
+    <t>Lecture 5: BLUES for Prediction and MVUE</t>
+  </si>
+  <si>
+    <t>05-BLUE-MVUE</t>
+  </si>
+  <si>
+    <t>Lecture 6: Generalized Linear Squares</t>
+  </si>
+  <si>
+    <t>06-GLS</t>
+  </si>
+  <si>
+    <t>07-sampling</t>
   </si>
 </sst>
 </file>
@@ -689,7 +707,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -821,8 +839,12 @@
       <c r="B8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="18">
@@ -830,8 +852,12 @@
       <c r="B9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -851,8 +877,12 @@
       <c r="B11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="18">

</xml_diff>

<commit_message>
lecture 7 sampling distributions
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD808D5-CD1F-6F4B-8E1A-27B3A8092B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BFD4E0-4128-B547-BE7A-F557328AD621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -314,9 +314,6 @@
     <t>04-BLUE</t>
   </si>
   <si>
-    <t>Lecture 7: Sampling Distributions</t>
-  </si>
-  <si>
     <t>Lecture 5: BLUES for Prediction and MVUE</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>07-sampling</t>
+  </si>
+  <si>
+    <t>Lecture 7: Sampling Distributions &amp; Distribution Theory</t>
   </si>
 </sst>
 </file>
@@ -707,7 +707,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -840,13 +840,13 @@
         <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
@@ -855,13 +855,13 @@
         <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -882,10 +882,10 @@
         <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update schedule for reading for Thursday
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A1A84-9C18-1948-8BE3-3D6793BBC672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888CB6EF-74F6-7A4C-886F-706FEFCAAF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
   <si>
     <t>Week</t>
   </si>
@@ -330,6 +330,12 @@
   </si>
   <si>
     <t>Lecture 7: Sampling Distributions &amp; Distribution Theory</t>
+  </si>
+  <si>
+    <t>Lecture 8: Bayesian Estimation</t>
+  </si>
+  <si>
+    <t>08-bayes</t>
   </si>
 </sst>
 </file>
@@ -707,7 +713,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -896,8 +902,12 @@
       <c r="B12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
upload lecture 8 bayes
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888CB6EF-74F6-7A4C-886F-706FEFCAAF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4176BFB-D175-3C45-B234-B005C984770C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6520" yWindow="3440" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
   <si>
     <t>Week</t>
   </si>
@@ -713,7 +713,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -908,7 +908,9 @@
       <c r="D12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
update calendar & hw
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A6B261-6C86-404C-A60B-D4FF97477A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F3BF4F-8DFD-8D46-945D-C26586733C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t>Week</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>14-testing-submodels</t>
+  </si>
+  <si>
+    <t>hw-12</t>
+  </si>
+  <si>
+    <t>Fri, Nov 22</t>
   </si>
 </sst>
 </file>
@@ -746,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1125,9 +1131,6 @@
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="G26" t="s">
-        <v>30</v>
-      </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
@@ -1137,6 +1140,9 @@
       </c>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
@@ -1156,9 +1162,6 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="G29" t="s">
-        <v>31</v>
-      </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="18">
@@ -1167,6 +1170,9 @@
         <v>62</v>
       </c>
       <c r="C30" s="2"/>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="18">
@@ -1186,9 +1192,6 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="G32" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
@@ -1197,6 +1200,9 @@
       </c>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
@@ -1214,9 +1220,6 @@
         <v>67</v>
       </c>
       <c r="C35" s="2"/>
-      <c r="G35" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
@@ -1227,6 +1230,9 @@
         <v>77</v>
       </c>
       <c r="E36" s="2"/>
+      <c r="G36" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
@@ -1252,42 +1258,52 @@
         <v>71</v>
       </c>
       <c r="C39" s="2"/>
+      <c r="G39" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="18">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="18">
+      <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" ht="18">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="18">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" ht="18">
-      <c r="A42" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18">
+      <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update to add LR
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F3BF4F-8DFD-8D46-945D-C26586733C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37B9718-53C8-2448-8E97-39A353F89EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
   <si>
     <t>Week</t>
   </si>
@@ -368,9 +368,6 @@
     <t>13-testing</t>
   </si>
   <si>
-    <t>Lec 14:  Testing Submodels</t>
-  </si>
-  <si>
     <t>14-testing-submodels</t>
   </si>
   <si>
@@ -378,6 +375,27 @@
   </si>
   <si>
     <t>Fri, Nov 22</t>
+  </si>
+  <si>
+    <t>Lec 15: Confidence Regions and Intervals</t>
+  </si>
+  <si>
+    <t>Lec 14: Testing Submodels</t>
+  </si>
+  <si>
+    <t>Lec 16:</t>
+  </si>
+  <si>
+    <t>Lec 17:</t>
+  </si>
+  <si>
+    <t>Lec 18:</t>
+  </si>
+  <si>
+    <t>Lec 19:</t>
+  </si>
+  <si>
+    <t>Review in Lab (see Canvas)</t>
   </si>
 </sst>
 </file>
@@ -754,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1072,13 +1090,13 @@
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G21" t="s">
         <v>29</v>
@@ -1090,7 +1108,9 @@
       <c r="B22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="23" spans="1:8" ht="18">
       <c r="A23" s="2" t="s">
@@ -1129,7 +1149,9 @@
       <c r="B26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -1138,7 +1160,9 @@
       <c r="B27" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
         <v>30</v>
@@ -1150,7 +1174,9 @@
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
@@ -1159,7 +1185,9 @@
       <c r="B29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="H29" s="2"/>
@@ -1169,7 +1197,9 @@
       <c r="B30" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="G30" t="s">
         <v>31</v>
       </c>
@@ -1259,13 +1289,13 @@
       </c>
       <c r="C39" s="2"/>
       <c r="G39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C40" s="2"/>
     </row>

</xml_diff>

<commit_message>
add Lec 15 CI
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37B9718-53C8-2448-8E97-39A353F89EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DABA581-15F5-7D41-97FB-27218A3E3FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
   <si>
     <t>Week</t>
   </si>
@@ -392,10 +393,16 @@
     <t>Lec 18:</t>
   </si>
   <si>
-    <t>Lec 19:</t>
-  </si>
-  <si>
     <t>Review in Lab (see Canvas)</t>
+  </si>
+  <si>
+    <t>15-CI</t>
+  </si>
+  <si>
+    <t>Lec 20:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 19: </t>
   </si>
 </sst>
 </file>
@@ -772,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1109,7 +1116,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1153,6 +1160,9 @@
         <v>113</v>
       </c>
       <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
@@ -1174,9 +1184,6 @@
       <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
@@ -1186,7 +1193,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1198,7 +1205,7 @@
         <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G30" t="s">
         <v>31</v>
@@ -1219,7 +1226,9 @@
       <c r="B32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
@@ -1228,7 +1237,9 @@
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="G33" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
add reading and fix title slide
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DABA581-15F5-7D41-97FB-27218A3E3FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057BD201-3942-2546-8B9F-8742741727B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
   <si>
     <t>Week</t>
   </si>
@@ -363,9 +363,6 @@
     <t>NO CLASS - Use time for review</t>
   </si>
   <si>
-    <t>Lec 13: Testing Hypotheses</t>
-  </si>
-  <si>
     <t>13-testing</t>
   </si>
   <si>
@@ -378,31 +375,34 @@
     <t>Fri, Nov 22</t>
   </si>
   <si>
-    <t>Lec 15: Confidence Regions and Intervals</t>
-  </si>
-  <si>
-    <t>Lec 14: Testing Submodels</t>
-  </si>
-  <si>
-    <t>Lec 16:</t>
-  </si>
-  <si>
-    <t>Lec 17:</t>
-  </si>
-  <si>
-    <t>Lec 18:</t>
-  </si>
-  <si>
     <t>Review in Lab (see Canvas)</t>
   </si>
   <si>
     <t>15-CI</t>
   </si>
   <si>
-    <t>Lec 20:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lec 19: </t>
+    <t>Lecture 15: Confidence Regions and Intervals</t>
+  </si>
+  <si>
+    <t>Lecture 13: Testing Hypotheses</t>
+  </si>
+  <si>
+    <t>Lecture 14: Testing Submodels</t>
+  </si>
+  <si>
+    <t>Lecture 16:</t>
+  </si>
+  <si>
+    <t>Lecture 17:</t>
+  </si>
+  <si>
+    <t>Lecture 18:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture 19: </t>
+  </si>
+  <si>
+    <t>Lecture 20:</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1081,13 +1081,13 @@
         <v>106</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1097,13 +1097,13 @@
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
         <v>29</v>
@@ -1116,7 +1116,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1157,11 +1157,13 @@
         <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1171,7 +1173,7 @@
         <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E27" s="2"/>
       <c r="G27" t="s">
@@ -1193,7 +1195,7 @@
         <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1205,7 +1207,7 @@
         <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G30" t="s">
         <v>31</v>
@@ -1227,7 +1229,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1238,7 +1240,7 @@
         <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E33" s="2"/>
       <c r="G33" t="s">
@@ -1300,13 +1302,13 @@
       </c>
       <c r="C39" s="2"/>
       <c r="G39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="2"/>
     </row>

</xml_diff>

<commit_message>
upload lecture 17 BMA
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6D83B9-1B92-354F-9B7E-BAE55E7073B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2539B8A0-4ABE-2345-AC4C-CF27CB392CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6520" yWindow="4920" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="124">
   <si>
     <t>Week</t>
   </si>
@@ -390,9 +389,6 @@
     <t>Lecture 14: Testing Submodels</t>
   </si>
   <si>
-    <t>Lecture 17:</t>
-  </si>
-  <si>
     <t>Lecture 18:</t>
   </si>
   <si>
@@ -406,6 +402,12 @@
   </si>
   <si>
     <t>16-Bayes-tests</t>
+  </si>
+  <si>
+    <t>Lecture 17: Bayesian Model Averaging</t>
+  </si>
+  <si>
+    <t>17-bma</t>
   </si>
 </sst>
 </file>
@@ -783,7 +785,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1176,13 +1178,13 @@
         <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" t="s">
         <v>121</v>
       </c>
-      <c r="D27" t="s">
-        <v>122</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -1203,10 +1205,14 @@
         <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+        <v>122</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="18">
@@ -1215,7 +1221,7 @@
         <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G30" t="s">
         <v>31</v>
@@ -1237,7 +1243,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1248,7 +1254,7 @@
         <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E33" s="2"/>
       <c r="G33" t="s">

</xml_diff>

<commit_message>
add reading and HW 9
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Library/Mobile Documents/com~apple~CloudDocs/Github/STA721-F24/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE4B45A-AD41-9A4C-AC0B-B304347897EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656C70F0-4F1E-FC4E-B857-67D40DCB0CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="4920" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6520" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="125">
   <si>
     <t>Week</t>
   </si>
@@ -272,9 +272,6 @@
     <t>Midterm2</t>
   </si>
   <si>
-    <t>hw-11</t>
-  </si>
-  <si>
     <t>Lecture 1:  Introduction to Linear Models</t>
   </si>
   <si>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>18-bvs</t>
+  </si>
+  <si>
+    <t>19-bvs</t>
   </si>
 </sst>
 </file>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -834,13 +834,13 @@
         <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
         <v>79</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
@@ -849,13 +849,13 @@
         <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -868,7 +868,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -879,13 +879,13 @@
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
@@ -894,13 +894,13 @@
         <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>24</v>
@@ -921,13 +921,13 @@
         <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
@@ -936,13 +936,13 @@
         <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>25</v>
@@ -963,13 +963,13 @@
         <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
@@ -978,13 +978,13 @@
         <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>26</v>
@@ -1005,13 +1005,13 @@
         <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
@@ -1020,13 +1020,13 @@
         <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
         <v>27</v>
@@ -1046,13 +1046,13 @@
         <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1062,13 +1062,13 @@
         <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G18" t="s">
         <v>28</v>
@@ -1086,16 +1086,16 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1105,13 +1105,13 @@
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
         <v>29</v>
@@ -1124,7 +1124,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1144,7 +1144,7 @@
         <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
@@ -1165,13 +1165,13 @@
         <v>58</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1181,13 +1181,13 @@
         <v>59</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
         <v>119</v>
       </c>
-      <c r="D27" t="s">
-        <v>120</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -1208,13 +1208,13 @@
         <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -1224,13 +1224,13 @@
         <v>62</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" t="s">
         <v>123</v>
       </c>
-      <c r="D30" t="s">
-        <v>124</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1240,9 +1240,6 @@
         <v>63</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="G31" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
@@ -1252,10 +1249,17 @@
         <v>64</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+        <v>116</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
@@ -1263,7 +1267,7 @@
         <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E33" s="2"/>
       <c r="H33" s="2"/>
@@ -1274,9 +1278,6 @@
         <v>66</v>
       </c>
       <c r="C34" s="2"/>
-      <c r="G34" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
@@ -1296,6 +1297,9 @@
         <v>77</v>
       </c>
       <c r="E36" s="2"/>
+      <c r="G36" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
@@ -1303,9 +1307,6 @@
         <v>69</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="G37" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
@@ -1328,9 +1329,12 @@
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="2"/>
+      <c r="G40" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2" t="s">
@@ -1342,9 +1346,6 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="G41" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>

</xml_diff>